<commit_message>
Generate figures and tables
</commit_message>
<xml_diff>
--- a/3.Results/Tables/Sheet S2.xlsx
+++ b/3.Results/Tables/Sheet S2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hu-my.sharepoint.com/personal/leacavalli_g_harvard_edu/Documents/Documents/GitHub/Calibration-Review/3.Results/Tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_DC7C157AC357CE84EA0B5B66425EAB250039451A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5B95916F-BBEF-478E-89AB-C1626A29E499}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="11_9B3C766BC357CE84EA0B5BFAF281801314C7E710" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B9349D6B-A13E-48E2-A233-1E94E6F0005C}"/>
   <bookViews>
-    <workbookView xWindow="37320" yWindow="-5490" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-6345" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 2" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="132">
   <si>
     <t>Field</t>
   </si>
@@ -308,9 +308,6 @@
   </si>
   <si>
     <t>Approximate Bayesian Computation Accept-Reject Random sampling (ABC-RS)</t>
-  </si>
-  <si>
-    <t>Bayesian history matching</t>
   </si>
   <si>
     <t>Coordinate descent algorithm</t>
@@ -790,15 +787,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D155"/>
+  <dimension ref="A1:D153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="B116" sqref="B116"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="B72" sqref="B72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="36.1796875" customWidth="1"/>
+    <col min="2" max="2" width="45.26953125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
@@ -823,10 +820,10 @@
         <v>27</v>
       </c>
       <c r="C2">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D2">
-        <v>17.5</v>
+        <v>17.399999999999999</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
@@ -840,7 +837,7 @@
         <v>60</v>
       </c>
       <c r="D3">
-        <v>14.2</v>
+        <v>14.299999999999999</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
@@ -851,10 +848,10 @@
         <v>29</v>
       </c>
       <c r="C4">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D4">
-        <v>18.399999999999999</v>
+        <v>18.099999999999998</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
@@ -868,7 +865,7 @@
         <v>77</v>
       </c>
       <c r="D5">
-        <v>18.2</v>
+        <v>18.399999999999999</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
@@ -879,10 +876,10 @@
         <v>31</v>
       </c>
       <c r="C6">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D6">
-        <v>17</v>
+        <v>16.900000000000002</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
@@ -896,7 +893,7 @@
         <v>60</v>
       </c>
       <c r="D7">
-        <v>14.2</v>
+        <v>14.299999999999999</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
@@ -921,10 +918,10 @@
         <v>34</v>
       </c>
       <c r="C9">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D9">
-        <v>50.8</v>
+        <v>51.1</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
@@ -935,10 +932,10 @@
         <v>35</v>
       </c>
       <c r="C10">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D10">
-        <v>16.5</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
@@ -952,7 +949,7 @@
         <v>149</v>
       </c>
       <c r="D11">
-        <v>35.199999999999996</v>
+        <v>35.6</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
@@ -963,10 +960,10 @@
         <v>37</v>
       </c>
       <c r="C12">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="D12">
-        <v>74</v>
+        <v>73.7</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
@@ -980,7 +977,7 @@
         <v>82</v>
       </c>
       <c r="D13">
-        <v>19.400000000000002</v>
+        <v>19.600000000000001</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
@@ -1008,7 +1005,7 @@
         <v>23</v>
       </c>
       <c r="D15">
-        <v>5.4</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
@@ -1022,7 +1019,7 @@
         <v>4</v>
       </c>
       <c r="D16">
-        <v>0.89999999999999991</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
@@ -1033,10 +1030,10 @@
         <v>42</v>
       </c>
       <c r="C17">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D17">
-        <v>35.5</v>
+        <v>35.6</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
@@ -1050,7 +1047,7 @@
         <v>91</v>
       </c>
       <c r="D18">
-        <v>21.5</v>
+        <v>21.7</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
@@ -1061,10 +1058,10 @@
         <v>40</v>
       </c>
       <c r="C19">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="D19">
-        <v>43</v>
+        <v>42.699999999999996</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
@@ -1078,7 +1075,7 @@
         <v>37</v>
       </c>
       <c r="D20">
-        <v>8.6999999999999993</v>
+        <v>8.7999999999999989</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
@@ -1089,10 +1086,10 @@
         <v>45</v>
       </c>
       <c r="C21">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="D21">
-        <v>71.399999999999991</v>
+        <v>71.099999999999994</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
@@ -1103,7 +1100,7 @@
         <v>46</v>
       </c>
       <c r="C22">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D22">
         <v>24.3</v>
@@ -1117,10 +1114,10 @@
         <v>47</v>
       </c>
       <c r="C23">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D23">
-        <v>38.299999999999997</v>
+        <v>38.4</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
@@ -1131,10 +1128,10 @@
         <v>48</v>
       </c>
       <c r="C24">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="D24">
-        <v>62.9</v>
+        <v>62.8</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
@@ -1159,10 +1156,10 @@
         <v>40</v>
       </c>
       <c r="C26">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D26">
-        <v>34</v>
+        <v>34.1</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
@@ -1176,7 +1173,7 @@
         <v>12</v>
       </c>
       <c r="D27">
-        <v>2.8000000000000003</v>
+        <v>2.9000000000000004</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
@@ -1187,10 +1184,10 @@
         <v>51</v>
       </c>
       <c r="C28">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="D28">
-        <v>91.7</v>
+        <v>91.600000000000009</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.35">
@@ -1204,7 +1201,7 @@
         <v>23</v>
       </c>
       <c r="D29">
-        <v>5.4</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.35">
@@ -1215,10 +1212,10 @@
         <v>52</v>
       </c>
       <c r="C30">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D30">
-        <v>14.399999999999999</v>
+        <v>14.299999999999999</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.35">
@@ -1229,10 +1226,10 @@
         <v>53</v>
       </c>
       <c r="C31">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D31">
-        <v>34</v>
+        <v>34.1</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.35">
@@ -1246,7 +1243,7 @@
         <v>25</v>
       </c>
       <c r="D32">
-        <v>5.8999999999999995</v>
+        <v>6</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.35">
@@ -1257,10 +1254,10 @@
         <v>55</v>
       </c>
       <c r="C33">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D33">
-        <v>45.4</v>
+        <v>45.300000000000004</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.35">
@@ -1288,7 +1285,7 @@
         <v>15</v>
       </c>
       <c r="D35">
-        <v>3.5000000000000004</v>
+        <v>3.5999999999999996</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.35">
@@ -1299,10 +1296,10 @@
         <v>57</v>
       </c>
       <c r="C36">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="D36">
-        <v>92.9</v>
+        <v>92.800000000000011</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.35">
@@ -1316,7 +1313,7 @@
         <v>15</v>
       </c>
       <c r="D37">
-        <v>3.5000000000000004</v>
+        <v>3.5999999999999996</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.35">
@@ -1327,10 +1324,10 @@
         <v>58</v>
       </c>
       <c r="C38">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D38">
-        <v>47.8</v>
+        <v>48</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.35">
@@ -1344,7 +1341,7 @@
         <v>193</v>
       </c>
       <c r="D39">
-        <v>45.6</v>
+        <v>46.1</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.35">
@@ -1355,10 +1352,10 @@
         <v>60</v>
       </c>
       <c r="C40">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D40">
-        <v>42.1</v>
+        <v>42</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.35">
@@ -1369,10 +1366,10 @@
         <v>61</v>
       </c>
       <c r="C41">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D41">
-        <v>39.5</v>
+        <v>39.4</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.35">
@@ -1383,10 +1380,10 @@
         <v>62</v>
       </c>
       <c r="C42">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D42">
-        <v>28.1</v>
+        <v>28.199999999999996</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.35">
@@ -1397,10 +1394,10 @@
         <v>63</v>
       </c>
       <c r="C43">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D43">
-        <v>15.6</v>
+        <v>15.299999999999999</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.35">
@@ -1411,10 +1408,10 @@
         <v>64</v>
       </c>
       <c r="C44">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D44">
-        <v>5.7</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.35">
@@ -1537,10 +1534,10 @@
         <v>71</v>
       </c>
       <c r="C53">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="D53">
-        <v>61.199999999999996</v>
+        <v>60.9</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.35">
@@ -1554,7 +1551,7 @@
         <v>104</v>
       </c>
       <c r="D54">
-        <v>24.6</v>
+        <v>24.8</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.35">
@@ -1568,7 +1565,7 @@
         <v>38</v>
       </c>
       <c r="D55">
-        <v>9</v>
+        <v>9.1</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.35">
@@ -1582,7 +1579,7 @@
         <v>22</v>
       </c>
       <c r="D56">
-        <v>5.2</v>
+        <v>5.3</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.35">
@@ -1593,10 +1590,10 @@
         <v>74</v>
       </c>
       <c r="C57">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="D57">
-        <v>71.399999999999991</v>
+        <v>71.599999999999994</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.35">
@@ -1621,10 +1618,10 @@
         <v>56</v>
       </c>
       <c r="C59">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D59">
-        <v>26.5</v>
+        <v>26.3</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.35">
@@ -1635,7 +1632,7 @@
         <v>75</v>
       </c>
       <c r="C60">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D60">
         <v>32.9</v>
@@ -1652,7 +1649,7 @@
         <v>96</v>
       </c>
       <c r="D61">
-        <v>22.7</v>
+        <v>22.900000000000002</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.35">
@@ -1663,10 +1660,10 @@
         <v>40</v>
       </c>
       <c r="C62">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="D62">
-        <v>44.4</v>
+        <v>44.2</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.35">
@@ -1677,10 +1674,10 @@
         <v>77</v>
       </c>
       <c r="C63">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D63">
-        <v>20.100000000000001</v>
+        <v>19.8</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.35">
@@ -1694,7 +1691,7 @@
         <v>67</v>
       </c>
       <c r="D64">
-        <v>15.8</v>
+        <v>16</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.35">
@@ -1705,10 +1702,10 @@
         <v>79</v>
       </c>
       <c r="C65">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D65">
-        <v>7.8</v>
+        <v>7.6</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.35">
@@ -1722,7 +1719,7 @@
         <v>30</v>
       </c>
       <c r="D66">
-        <v>7.1</v>
+        <v>7.1999999999999993</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.35">
@@ -1736,7 +1733,7 @@
         <v>20</v>
       </c>
       <c r="D67">
-        <v>4.7</v>
+        <v>4.8</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.35">
@@ -1750,7 +1747,7 @@
         <v>15</v>
       </c>
       <c r="D68">
-        <v>3.5000000000000004</v>
+        <v>3.5999999999999996</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.35">
@@ -1764,7 +1761,7 @@
         <v>12</v>
       </c>
       <c r="D69">
-        <v>2.8000000000000003</v>
+        <v>2.9000000000000004</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.35">
@@ -1803,10 +1800,10 @@
         <v>86</v>
       </c>
       <c r="C72">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D72">
-        <v>1.4000000000000001</v>
+        <v>1.7000000000000002</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.35">
@@ -2097,10 +2094,10 @@
         <v>107</v>
       </c>
       <c r="C93">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="D93">
-        <v>0.2</v>
+        <v>5.7</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.35">
@@ -2108,27 +2105,27 @@
         <v>17</v>
       </c>
       <c r="B94" t="s">
-        <v>108</v>
+        <v>40</v>
       </c>
       <c r="C94">
-        <v>24</v>
+        <v>98</v>
       </c>
       <c r="D94">
-        <v>5.7</v>
+        <v>23.400000000000002</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B95" t="s">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="C95">
-        <v>99</v>
+        <v>83</v>
       </c>
       <c r="D95">
-        <v>23.400000000000002</v>
+        <v>19.8</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.35">
@@ -2136,13 +2133,13 @@
         <v>18</v>
       </c>
       <c r="B96" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C96">
-        <v>85</v>
+        <v>67</v>
       </c>
       <c r="D96">
-        <v>20.100000000000001</v>
+        <v>16</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.35">
@@ -2150,13 +2147,13 @@
         <v>18</v>
       </c>
       <c r="B97" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C97">
-        <v>67</v>
+        <v>40</v>
       </c>
       <c r="D97">
-        <v>15.8</v>
+        <v>9.5</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.35">
@@ -2164,13 +2161,13 @@
         <v>18</v>
       </c>
       <c r="B98" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C98">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="D98">
-        <v>9.5</v>
+        <v>7.6</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.35">
@@ -2178,13 +2175,13 @@
         <v>18</v>
       </c>
       <c r="B99" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C99">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="D99">
-        <v>7.8</v>
+        <v>4.8</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.35">
@@ -2192,13 +2189,13 @@
         <v>18</v>
       </c>
       <c r="B100" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C100">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D100">
-        <v>4.7</v>
+        <v>3.5999999999999996</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.35">
@@ -2206,13 +2203,13 @@
         <v>18</v>
       </c>
       <c r="B101" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C101">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D101">
-        <v>3.5000000000000004</v>
+        <v>2.9000000000000004</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.35">
@@ -2220,13 +2217,13 @@
         <v>18</v>
       </c>
       <c r="B102" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C102">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D102">
-        <v>2.8000000000000003</v>
+        <v>2.1</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.35">
@@ -2234,13 +2231,13 @@
         <v>18</v>
       </c>
       <c r="B103" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C103">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D103">
-        <v>2.1</v>
+        <v>1.7000000000000002</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.35">
@@ -2248,7 +2245,7 @@
         <v>18</v>
       </c>
       <c r="B104" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C104">
         <v>6</v>
@@ -2262,13 +2259,13 @@
         <v>18</v>
       </c>
       <c r="B105" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C105">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D105">
-        <v>1.4000000000000001</v>
+        <v>0.70000000000000007</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.35">
@@ -2276,7 +2273,7 @@
         <v>18</v>
       </c>
       <c r="B106" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C106">
         <v>3</v>
@@ -2290,13 +2287,13 @@
         <v>18</v>
       </c>
       <c r="B107" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C107">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D107">
-        <v>0.70000000000000007</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.35">
@@ -2304,7 +2301,7 @@
         <v>18</v>
       </c>
       <c r="B108" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C108">
         <v>2</v>
@@ -2318,7 +2315,7 @@
         <v>18</v>
       </c>
       <c r="B109" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C109">
         <v>2</v>
@@ -2332,13 +2329,13 @@
         <v>18</v>
       </c>
       <c r="B110" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="C110">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D110">
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.35">
@@ -2346,7 +2343,7 @@
         <v>18</v>
       </c>
       <c r="B111" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C111">
         <v>1</v>
@@ -2360,7 +2357,7 @@
         <v>18</v>
       </c>
       <c r="B112" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C112">
         <v>1</v>
@@ -2374,7 +2371,7 @@
         <v>18</v>
       </c>
       <c r="B113" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C113">
         <v>1</v>
@@ -2388,7 +2385,7 @@
         <v>18</v>
       </c>
       <c r="B114" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C114">
         <v>1</v>
@@ -2402,7 +2399,7 @@
         <v>18</v>
       </c>
       <c r="B115" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C115">
         <v>1</v>
@@ -2416,7 +2413,7 @@
         <v>18</v>
       </c>
       <c r="B116" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C116">
         <v>1</v>
@@ -2430,7 +2427,7 @@
         <v>18</v>
       </c>
       <c r="B117" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C117">
         <v>1</v>
@@ -2444,7 +2441,7 @@
         <v>18</v>
       </c>
       <c r="B118" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C118">
         <v>1</v>
@@ -2458,7 +2455,7 @@
         <v>18</v>
       </c>
       <c r="B119" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C119">
         <v>1</v>
@@ -2472,7 +2469,7 @@
         <v>18</v>
       </c>
       <c r="B120" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C120">
         <v>1</v>
@@ -2486,13 +2483,13 @@
         <v>18</v>
       </c>
       <c r="B121" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C121">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="D121">
-        <v>0.2</v>
+        <v>5.7</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.35">
@@ -2500,41 +2497,41 @@
         <v>18</v>
       </c>
       <c r="B122" t="s">
-        <v>107</v>
+        <v>40</v>
       </c>
       <c r="C122">
-        <v>1</v>
+        <v>98</v>
       </c>
       <c r="D122">
-        <v>0.2</v>
+        <v>23.400000000000002</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B123" t="s">
         <v>108</v>
       </c>
       <c r="C123">
-        <v>24</v>
+        <v>82</v>
       </c>
       <c r="D123">
-        <v>5.7</v>
+        <v>19.600000000000001</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B124" t="s">
-        <v>40</v>
+        <v>109</v>
       </c>
       <c r="C124">
-        <v>99</v>
+        <v>9</v>
       </c>
       <c r="D124">
-        <v>23.400000000000002</v>
+        <v>2.1</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.35">
@@ -2542,41 +2539,41 @@
         <v>19</v>
       </c>
       <c r="B125" t="s">
-        <v>109</v>
+        <v>55</v>
       </c>
       <c r="C125">
-        <v>82</v>
+        <v>328</v>
       </c>
       <c r="D125">
-        <v>19.400000000000002</v>
+        <v>78.3</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B126" t="s">
         <v>110</v>
       </c>
       <c r="C126">
-        <v>9</v>
+        <v>115</v>
       </c>
       <c r="D126">
-        <v>2.1</v>
+        <v>27.400000000000002</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B127" t="s">
-        <v>55</v>
+        <v>111</v>
       </c>
       <c r="C127">
-        <v>332</v>
+        <v>93</v>
       </c>
       <c r="D127">
-        <v>78.5</v>
+        <v>22.2</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.35">
@@ -2584,13 +2581,13 @@
         <v>20</v>
       </c>
       <c r="B128" t="s">
-        <v>111</v>
+        <v>40</v>
       </c>
       <c r="C128">
-        <v>116</v>
+        <v>181</v>
       </c>
       <c r="D128">
-        <v>27.400000000000002</v>
+        <v>43.2</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.35">
@@ -2601,10 +2598,10 @@
         <v>112</v>
       </c>
       <c r="C129">
-        <v>94</v>
+        <v>8</v>
       </c>
       <c r="D129">
-        <v>22.2</v>
+        <v>1.9</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.35">
@@ -2612,41 +2609,41 @@
         <v>20</v>
       </c>
       <c r="B130" t="s">
-        <v>40</v>
+        <v>107</v>
       </c>
       <c r="C130">
-        <v>183</v>
+        <v>22</v>
       </c>
       <c r="D130">
-        <v>43.3</v>
+        <v>5.3</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B131" t="s">
         <v>113</v>
       </c>
       <c r="C131">
-        <v>8</v>
+        <v>110</v>
       </c>
       <c r="D131">
-        <v>1.9</v>
+        <v>26.3</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B132" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="C132">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D132">
-        <v>5.2</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.35">
@@ -2654,13 +2651,13 @@
         <v>21</v>
       </c>
       <c r="B133" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C133">
-        <v>110</v>
+        <v>84</v>
       </c>
       <c r="D133">
-        <v>26</v>
+        <v>20</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.35">
@@ -2668,13 +2665,13 @@
         <v>21</v>
       </c>
       <c r="B134" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C134">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="D134">
-        <v>5.4</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.35">
@@ -2682,13 +2679,13 @@
         <v>21</v>
       </c>
       <c r="B135" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C135">
-        <v>85</v>
+        <v>33</v>
       </c>
       <c r="D135">
-        <v>20.100000000000001</v>
+        <v>7.9</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.35">
@@ -2696,13 +2693,13 @@
         <v>21</v>
       </c>
       <c r="B136" t="s">
-        <v>117</v>
+        <v>40</v>
       </c>
       <c r="C136">
-        <v>1</v>
+        <v>181</v>
       </c>
       <c r="D136">
-        <v>0.2</v>
+        <v>43.2</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.35">
@@ -2710,69 +2707,69 @@
         <v>21</v>
       </c>
       <c r="B137" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
       <c r="C137">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="D137">
-        <v>7.8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B138" t="s">
-        <v>40</v>
+        <v>118</v>
       </c>
       <c r="C138">
-        <v>184</v>
+        <v>100</v>
       </c>
       <c r="D138">
-        <v>43.5</v>
+        <v>23.9</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B139" t="s">
-        <v>108</v>
+        <v>119</v>
       </c>
       <c r="C139">
-        <v>21</v>
+        <v>319</v>
       </c>
       <c r="D139">
-        <v>5</v>
+        <v>76.099999999999994</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B140" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C140">
-        <v>101</v>
+        <v>174</v>
       </c>
       <c r="D140">
-        <v>23.9</v>
+        <v>41.5</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B141" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C141">
-        <v>322</v>
+        <v>189</v>
       </c>
       <c r="D141">
-        <v>76.099999999999994</v>
+        <v>45.1</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.35">
@@ -2780,13 +2777,13 @@
         <v>23</v>
       </c>
       <c r="B142" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C142">
-        <v>178</v>
+        <v>1</v>
       </c>
       <c r="D142">
-        <v>42.1</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.35">
@@ -2794,41 +2791,41 @@
         <v>23</v>
       </c>
       <c r="B143" t="s">
-        <v>122</v>
+        <v>55</v>
       </c>
       <c r="C143">
-        <v>189</v>
+        <v>55</v>
       </c>
       <c r="D143">
-        <v>44.7</v>
+        <v>13.100000000000001</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B144" t="s">
         <v>123</v>
       </c>
       <c r="C144">
-        <v>1</v>
+        <v>40</v>
       </c>
       <c r="D144">
-        <v>0.2</v>
+        <v>9.5</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B145" t="s">
-        <v>55</v>
+        <v>124</v>
       </c>
       <c r="C145">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D145">
-        <v>13</v>
+        <v>12.6</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.35">
@@ -2836,13 +2833,13 @@
         <v>24</v>
       </c>
       <c r="B146" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C146">
-        <v>41</v>
+        <v>311</v>
       </c>
       <c r="D146">
-        <v>9.7000000000000011</v>
+        <v>74.2</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.35">
@@ -2850,41 +2847,41 @@
         <v>24</v>
       </c>
       <c r="B147" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C147">
-        <v>54</v>
+        <v>15</v>
       </c>
       <c r="D147">
-        <v>12.8</v>
+        <v>3.5999999999999996</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B148" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C148">
-        <v>313</v>
+        <v>52</v>
       </c>
       <c r="D148">
-        <v>74</v>
+        <v>12.4</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B149" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C149">
-        <v>15</v>
+        <v>64</v>
       </c>
       <c r="D149">
-        <v>3.5000000000000004</v>
+        <v>15.299999999999999</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.35">
@@ -2892,13 +2889,13 @@
         <v>25</v>
       </c>
       <c r="B150" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C150">
-        <v>52</v>
+        <v>170</v>
       </c>
       <c r="D150">
-        <v>12.3</v>
+        <v>40.6</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.35">
@@ -2906,69 +2903,41 @@
         <v>25</v>
       </c>
       <c r="B151" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C151">
-        <v>65</v>
+        <v>133</v>
       </c>
       <c r="D151">
-        <v>15.4</v>
+        <v>31.7</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B152" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C152">
-        <v>170</v>
+        <v>309</v>
       </c>
       <c r="D152">
-        <v>40.200000000000003</v>
+        <v>73.7</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B153" t="s">
-        <v>131</v>
+        <v>40</v>
       </c>
       <c r="C153">
-        <v>136</v>
+        <v>110</v>
       </c>
       <c r="D153">
-        <v>32.200000000000003</v>
-      </c>
-    </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A154" t="s">
-        <v>26</v>
-      </c>
-      <c r="B154" t="s">
-        <v>132</v>
-      </c>
-      <c r="C154">
-        <v>311</v>
-      </c>
-      <c r="D154">
-        <v>73.5</v>
-      </c>
-    </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A155" t="s">
-        <v>26</v>
-      </c>
-      <c r="B155" t="s">
-        <v>40</v>
-      </c>
-      <c r="C155">
-        <v>112</v>
-      </c>
-      <c r="D155">
-        <v>26.5</v>
+        <v>26.3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>